<commit_message>
Corrected unit of investments
From mio€ to €
</commit_message>
<xml_diff>
--- a/import/raw_data/e3m/investments_per_ktoe_updated.xlsx
+++ b/import/raw_data/e3m/investments_per_ktoe_updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\e3m\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BE714B-45D9-4048-B21A-B7EADC648E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFAD5CD-B9D4-4CE6-9690-4EE17151DE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="28980" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,37 +429,37 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>10.42</v>
+        <v>10420000</v>
       </c>
       <c r="D2">
-        <v>12.72</v>
+        <v>12720000</v>
       </c>
       <c r="E2">
-        <v>15.54</v>
+        <v>15540000</v>
       </c>
       <c r="F2">
-        <v>18.98</v>
+        <v>18980000</v>
       </c>
       <c r="G2">
-        <v>21.872441605782164</v>
+        <v>21872441.605782162</v>
       </c>
       <c r="H2">
-        <v>29.269337274300366</v>
+        <v>29269337.274300367</v>
       </c>
       <c r="I2">
-        <v>35.65121750462788</v>
+        <v>35651217.504627883</v>
       </c>
       <c r="J2">
-        <v>41.657693015524366</v>
+        <v>41657693.015524365</v>
       </c>
       <c r="K2">
-        <v>49.992089914467037</v>
+        <v>49992089.914467037</v>
       </c>
       <c r="L2">
-        <v>61.573177227539965</v>
+        <v>61573177.227539964</v>
       </c>
       <c r="M2">
-        <v>77.133842768511997</v>
+        <v>77133842.768511996</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -470,37 +470,37 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>4.2814045303986967</v>
+        <v>4281404.5303986967</v>
       </c>
       <c r="D3">
-        <v>5.2264362405634763</v>
+        <v>5226436.2405634765</v>
       </c>
       <c r="E3">
-        <v>6.3851272938959438</v>
+        <v>6385127.293895944</v>
       </c>
       <c r="F3">
-        <v>7.7985660256206577</v>
+        <v>7798566.025620658</v>
       </c>
       <c r="G3">
-        <v>8.9870221287789533</v>
+        <v>8987022.1287789531</v>
       </c>
       <c r="H3">
-        <v>12.026283417270347</v>
+        <v>12026283.417270347</v>
       </c>
       <c r="I3">
-        <v>14.64849175993696</v>
+        <v>14648491.75993696</v>
       </c>
       <c r="J3">
-        <v>17.116452553034947</v>
+        <v>17116452.553034946</v>
       </c>
       <c r="K3">
-        <v>20.540917489817481</v>
+        <v>20540917.489817481</v>
       </c>
       <c r="L3">
-        <v>25.299393467661368</v>
+        <v>25299393.467661366</v>
       </c>
       <c r="M3">
-        <v>31.693011888307868</v>
+        <v>31693011.888307869</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -511,37 +511,37 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>3.9784418079170281</v>
+        <v>3978441.8079170282</v>
       </c>
       <c r="D4">
-        <v>4.8566007482442028</v>
+        <v>4856600.7482442027</v>
       </c>
       <c r="E4">
-        <v>5.9332999707323042</v>
+        <v>5933299.9707323043</v>
       </c>
       <c r="F4">
-        <v>7.2467202988738189</v>
+        <v>7246720.2988738185</v>
       </c>
       <c r="G4">
-        <v>8.3510783230007313</v>
+        <v>8351078.3230007309</v>
       </c>
       <c r="H4">
-        <v>11.175274002120998</v>
+        <v>11175274.002120998</v>
       </c>
       <c r="I4">
-        <v>13.611928428364198</v>
+        <v>13611928.428364199</v>
       </c>
       <c r="J4">
-        <v>15.905250241298974</v>
+        <v>15905250.241298974</v>
       </c>
       <c r="K4">
-        <v>19.087391610447494</v>
+        <v>19087391.610447492</v>
       </c>
       <c r="L4">
-        <v>23.509146115962544</v>
+        <v>23509146.115962543</v>
       </c>
       <c r="M4">
-        <v>29.450336360417147</v>
+        <v>29450336.360417146</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -552,37 +552,37 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>7.7427982972823752</v>
+        <v>7742798.2972823754</v>
       </c>
       <c r="D5">
-        <v>9.4518612611738764</v>
+        <v>9451861.261173876</v>
       </c>
       <c r="E5">
-        <v>11.547321069075632</v>
+        <v>11547321.069075633</v>
       </c>
       <c r="F5">
-        <v>14.103484806374226</v>
+        <v>14103484.806374226</v>
       </c>
       <c r="G5">
-        <v>16.252773860139953</v>
+        <v>16252773.860139953</v>
       </c>
       <c r="H5">
-        <v>21.749191440502532</v>
+        <v>21749191.440502532</v>
       </c>
       <c r="I5">
-        <v>26.491380632521718</v>
+        <v>26491380.632521719</v>
       </c>
       <c r="J5">
-        <v>30.954617519128011</v>
+        <v>30954617.51912801</v>
       </c>
       <c r="K5">
-        <v>37.147664939282407</v>
+        <v>37147664.93928241</v>
       </c>
       <c r="L5">
-        <v>45.753233377702713</v>
+        <v>45753233.377702713</v>
       </c>
       <c r="M5">
-        <v>57.315910407954028</v>
+        <v>57315910.40795403</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -593,37 +593,37 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>3.6163692471481559</v>
+        <v>3616369.2471481557</v>
       </c>
       <c r="D6">
-        <v>4.4146081404726054</v>
+        <v>4414608.1404726058</v>
       </c>
       <c r="E6">
-        <v>5.3933184357660595</v>
+        <v>5393318.4357660599</v>
       </c>
       <c r="F6">
-        <v>6.5872061718687149</v>
+        <v>6587206.1718687145</v>
       </c>
       <c r="G6">
-        <v>7.5910580790013871</v>
+        <v>7591058.0790013866</v>
       </c>
       <c r="H6">
-        <v>10.1582275626859</v>
+        <v>10158227.562685899</v>
       </c>
       <c r="I6">
-        <v>12.373125394157993</v>
+        <v>12373125.394157993</v>
       </c>
       <c r="J6">
-        <v>14.457735117896435</v>
+        <v>14457735.117896436</v>
       </c>
       <c r="K6">
-        <v>17.350274142739359</v>
+        <v>17350274.142739359</v>
       </c>
       <c r="L6">
-        <v>21.369610803731163</v>
+        <v>21369610.803731162</v>
       </c>
       <c r="M6">
-        <v>26.770101430173511</v>
+        <v>26770101.430173513</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -716,37 +716,37 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>5.0215787849339071</v>
+        <v>5021578.784933907</v>
       </c>
       <c r="D9">
-        <v>5.9372158509379549</v>
+        <v>5937215.8509379551</v>
       </c>
       <c r="E9">
-        <v>7.1047563789087302</v>
+        <v>7104756.3789087301</v>
       </c>
       <c r="F9">
-        <v>8.5573712783534575</v>
+        <v>8557371.2783534583</v>
       </c>
       <c r="G9">
-        <v>10.540709092351385</v>
+        <v>10540709.092351384</v>
       </c>
       <c r="H9">
-        <v>13.66182179335104</v>
+        <v>13661821.793351039</v>
       </c>
       <c r="I9">
-        <v>16.299434683517859</v>
+        <v>16299434.683517858</v>
       </c>
       <c r="J9">
-        <v>18.781893874263101</v>
+        <v>18781893.8742631</v>
       </c>
       <c r="K9">
-        <v>22.178792422772915</v>
+        <v>22178792.422772914</v>
       </c>
       <c r="L9">
-        <v>26.823412234322308</v>
+        <v>26823412.234322309</v>
       </c>
       <c r="M9">
-        <v>32.951357238658211</v>
+        <v>32951357.238658212</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -757,37 +757,37 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>0.6172465409147414</v>
+        <v>617246.54091474146</v>
       </c>
       <c r="D10">
-        <v>0.72979556900526843</v>
+        <v>729795.56900526839</v>
       </c>
       <c r="E10">
-        <v>0.8733082735016926</v>
+        <v>873308.27350169257</v>
       </c>
       <c r="F10">
-        <v>1.0518619834730625</v>
+        <v>1051861.9834730625</v>
       </c>
       <c r="G10">
-        <v>1.2956515280737728</v>
+        <v>1295651.5280737728</v>
       </c>
       <c r="H10">
-        <v>1.679295019693801</v>
+        <v>1679295.0196938009</v>
       </c>
       <c r="I10">
-        <v>2.0035072848905982</v>
+        <v>2003507.2848905982</v>
       </c>
       <c r="J10">
-        <v>2.3086482403699367</v>
+        <v>2308648.2403699365</v>
       </c>
       <c r="K10">
-        <v>2.726191003055793</v>
+        <v>2726191.0030557928</v>
       </c>
       <c r="L10">
-        <v>3.2971021916135315</v>
+        <v>3297102.1916135317</v>
       </c>
       <c r="M10">
-        <v>4.0503419631751143</v>
+        <v>4050341.9631751142</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -798,37 +798,37 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>0.84805749493941496</v>
+        <v>848057.4949394149</v>
       </c>
       <c r="D11">
-        <v>1.0026927022568459</v>
+        <v>1002692.7022568459</v>
       </c>
       <c r="E11">
-        <v>1.1998700318970441</v>
+        <v>1199870.031897044</v>
       </c>
       <c r="F11">
-        <v>1.4451914747131562</v>
+        <v>1445191.4747131562</v>
       </c>
       <c r="G11">
-        <v>1.7801428057973374</v>
+        <v>1780142.8057973373</v>
       </c>
       <c r="H11">
-        <v>2.3072445664178662</v>
+        <v>2307244.5664178664</v>
       </c>
       <c r="I11">
-        <v>2.7526916013157212</v>
+        <v>2752691.6013157214</v>
       </c>
       <c r="J11">
-        <v>3.1719358694548792</v>
+        <v>3171935.8694548793</v>
       </c>
       <c r="K11">
-        <v>3.7456130727789896</v>
+        <v>3745613.0727789896</v>
       </c>
       <c r="L11">
-        <v>4.5300087401627884</v>
+        <v>4530008.7401627889</v>
       </c>
       <c r="M11">
-        <v>5.5649122858555424</v>
+        <v>5564912.2858555429</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -839,37 +839,37 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>0.74203912147950257</v>
+        <v>742039.12147950253</v>
       </c>
       <c r="D12">
-        <v>0.87734288811365602</v>
+        <v>877342.88811365596</v>
       </c>
       <c r="E12">
-        <v>1.0498704506138135</v>
+        <v>1049870.4506138135</v>
       </c>
       <c r="F12">
-        <v>1.2645234770815024</v>
+        <v>1264523.4770815023</v>
       </c>
       <c r="G12">
-        <v>1.5576014734900498</v>
+        <v>1557601.4734900498</v>
       </c>
       <c r="H12">
-        <v>2.0188085611169315</v>
+        <v>2018808.5611169315</v>
       </c>
       <c r="I12">
-        <v>2.408568840831065</v>
+        <v>2408568.8408310651</v>
       </c>
       <c r="J12">
-        <v>2.7754020452678967</v>
+        <v>2775402.0452678967</v>
       </c>
       <c r="K12">
-        <v>3.2773620308911027</v>
+        <v>3277362.0308911027</v>
       </c>
       <c r="L12">
-        <v>3.9636978930125544</v>
+        <v>3963697.8930125544</v>
       </c>
       <c r="M12">
-        <v>4.8692248442444805</v>
+        <v>4869224.8442444801</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -880,37 +880,37 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>10.524675265498784</v>
+        <v>10524675.265498783</v>
       </c>
       <c r="D13">
-        <v>11.488011212506617</v>
+        <v>11488011.212506616</v>
       </c>
       <c r="E13">
-        <v>13.039765876081933</v>
+        <v>13039765.876081934</v>
       </c>
       <c r="F13">
-        <v>15.122578403451879</v>
+        <v>15122578.403451879</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>26.434471288506323</v>
+        <v>26434471.288506322</v>
       </c>
       <c r="I13">
-        <v>29.915285035882984</v>
+        <v>29915285.035882983</v>
       </c>
       <c r="J13">
-        <v>33.19134503341396</v>
+        <v>33191345.033413962</v>
       </c>
       <c r="K13">
-        <v>37.507700189227208</v>
+        <v>37507700.189227208</v>
       </c>
       <c r="L13">
-        <v>43.155533046498775</v>
+        <v>43155533.046498775</v>
       </c>
       <c r="M13">
-        <v>50.244557034545878</v>
+        <v>50244557.034545876</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -921,37 +921,37 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>3.4274501444795007</v>
+        <v>3427450.1444795006</v>
       </c>
       <c r="D14">
-        <v>3.648731005152579</v>
+        <v>3648731.0051525789</v>
       </c>
       <c r="E14">
-        <v>4.0724687463955798</v>
+        <v>4072468.7463955795</v>
       </c>
       <c r="F14">
-        <v>4.6628700821815965</v>
+        <v>4662870.0821815962</v>
       </c>
       <c r="G14">
-        <v>7.1945012612147341</v>
+        <v>7194501.2612147341</v>
       </c>
       <c r="H14">
-        <v>8.3959071079408663</v>
+        <v>8395907.1079408657</v>
       </c>
       <c r="I14">
-        <v>9.3428873268048935</v>
+        <v>9342887.3268048931</v>
       </c>
       <c r="J14">
-        <v>10.234162826912213</v>
+        <v>10234162.826912213</v>
       </c>
       <c r="K14">
-        <v>11.393518783888167</v>
+        <v>11393518.783888167</v>
       </c>
       <c r="L14">
-        <v>12.888003328196765</v>
+        <v>12888003.328196766</v>
       </c>
       <c r="M14">
-        <v>14.732202216066417</v>
+        <v>14732202.216066416</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1044,37 +1044,37 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>7.2596360069645947</v>
+        <v>7259636.0069645951</v>
       </c>
       <c r="D17">
-        <v>7.7283280188328956</v>
+        <v>7728328.0188328959</v>
       </c>
       <c r="E17">
-        <v>8.6258412237418707</v>
+        <v>8625841.2237418704</v>
       </c>
       <c r="F17">
-        <v>9.8763623444460364</v>
+        <v>9876362.344446037</v>
       </c>
       <c r="G17">
-        <v>15.238576261186823</v>
+        <v>15238576.261186823</v>
       </c>
       <c r="H17">
-        <v>17.783257810506726</v>
+        <v>17783257.810506724</v>
       </c>
       <c r="I17">
-        <v>19.78904386280611</v>
+        <v>19789043.862806112</v>
       </c>
       <c r="J17">
-        <v>21.676842500264357</v>
+        <v>21676842.500264358</v>
       </c>
       <c r="K17">
-        <v>24.132458744225705</v>
+        <v>24132458.744225703</v>
       </c>
       <c r="L17">
-        <v>27.297906337151197</v>
+        <v>27297906.337151196</v>
       </c>
       <c r="M17">
-        <v>31.204079172938933</v>
+        <v>31204079.172938932</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1085,37 +1085,37 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <v>12.586899179357296</v>
+        <v>12586899.179357296</v>
       </c>
       <c r="D18">
-        <v>13.399526574711114</v>
+        <v>13399526.574711114</v>
       </c>
       <c r="E18">
-        <v>14.955652558368326</v>
+        <v>14955652.558368327</v>
       </c>
       <c r="F18">
-        <v>17.12383058449247</v>
+        <v>17123830.584492471</v>
       </c>
       <c r="G18">
-        <v>26.420942159151622</v>
+        <v>26420942.159151621</v>
       </c>
       <c r="H18">
-        <v>30.832960898676909</v>
+        <v>30832960.89867691</v>
       </c>
       <c r="I18">
-        <v>34.310632064480934</v>
+        <v>34310632.064480938</v>
       </c>
       <c r="J18">
-        <v>37.583734338178843</v>
+        <v>37583734.338178843</v>
       </c>
       <c r="K18">
-        <v>41.841329905819023</v>
+        <v>41841329.905819021</v>
       </c>
       <c r="L18">
-        <v>47.329644977190164</v>
+        <v>47329644.977190167</v>
       </c>
       <c r="M18">
-        <v>54.102243990974877</v>
+        <v>54102243.990974873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>